<commit_message>
also done with main_initiate now (there may be a bug, but i dont know)
</commit_message>
<xml_diff>
--- a/data/Min/Feriekasse.xlsx
+++ b/data/Min/Feriekasse.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,10 +424,40 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>op</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
+        <is>
+          <t>Point:</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Mads</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Point:</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Soren</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Point:</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Emil</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>Point:</t>
         </is>
@@ -436,66 +466,228 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Manchester City</t>
+          <t>Chelsea</t>
         </is>
       </c>
       <c r="B2">
-        <f>0</f>
+        <f>0+5+10+5+10+10+5+5+5+5+10+5+20+30+10+10+5+10</f>
+        <v/>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="D2">
+        <f>0+15+30+30+5+5+25+20+10+10+5+15+20+10+10+40+15</f>
+        <v/>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Manchester Utd</t>
+        </is>
+      </c>
+      <c r="F2">
+        <f>0+5+10+5+30+30+15+20+10+5+10+5+5+5+5+20+10+10+25+30+10+25+10</f>
+        <v/>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Leicester City</t>
+        </is>
+      </c>
+      <c r="H2">
+        <f>0+20+10+10+5+5+30+5+40+5+10+20+0+5+15+5+10+30+10+10+5+5+0+10+10</f>
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>0+10+10+20+5+5+10+30+30+10+5+15+10+5+10+10+15+5</f>
+        <v/>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Eint Frankfurt</t>
+        </is>
+      </c>
+      <c r="D3">
+        <f>0+40+5+5+5+5+5+10+15+10+0+20+5+15+15+10+10+10+5+10+15+0+0+30+5+5</f>
+        <v/>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Leverkusen</t>
         </is>
       </c>
-      <c r="B3">
-        <f>0</f>
+      <c r="F3">
+        <f>0+5+20+25+5+15+5+40+10+10+5+10+5+10+5+20</f>
+        <v/>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="H3">
+        <f>0+20+40+30+10+40+5+5+5+30+10+15+10+20+10+5+5</f>
         <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="B4">
-        <f>0</f>
+        <f>0+5+5+5+15+10+10+5+5+10+5+10+5+5+10+10+5+15</f>
+        <v/>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Hoffenheim</t>
+        </is>
+      </c>
+      <c r="D4">
+        <f>0+5+20+15+5+15+25+15+10+5+10+20+15+5+20+10+40+5+10+30+25</f>
+        <v/>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="F4">
+        <f>0+5+10+10+5+5+10+10+10+5+5+5+5+5+10+20+10+5+5+5+5</f>
+        <v/>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Dortmund</t>
+        </is>
+      </c>
+      <c r="H4">
+        <f>0+10+10+20+10+5+10+40+5+5+40+15+10</f>
         <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Bologna</t>
         </is>
       </c>
       <c r="B5">
-        <f>0</f>
+        <f>0+10+30+5+15+5+30+20+10+10+20+30+10+15+10+5+20+5+10+10+20+10+10+5+5+10+15</f>
+        <v/>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="D5">
+        <f>0+5+10+30+5+5+30+5+20+5+10+5+10+20+10+10+10+10+40+5+5+5+10+15+5+5+20+5</f>
+        <v/>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="F5">
+        <f>0+5+10+10+10+0+5+10+10+20+5+5+10+10+0+0+10+10+10+5+15</f>
+        <v/>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="H5">
+        <f>0+30+10+5+5+5+10+10+15+25+15+5+5+10+25+20+10+5+20+5+10+10</f>
         <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>AGF</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>0+10+5+10+15+30+15+0+0+50+10+0+0+10+5+10+10+10+5+5+5+15+10+0+0+5+10+10+5</f>
+        <v/>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Milan</t>
         </is>
       </c>
-      <c r="B6">
-        <f>0</f>
+      <c r="D6">
+        <f>0+10+5+10+15+5+10+10+10+5+5+10+10</f>
+        <v/>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="F6">
+        <f>0+20+10+5+5+10+20+10+10+5+5+10+5+15+10+10+10+5+10+10+5+10+10+20</f>
+        <v/>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="H6">
+        <f>0+10+10+5+20+5+5+20+5+5+5+10+10+10+10+5+15+10+10+10+5+30+10</f>
         <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Odense</t>
+        </is>
+      </c>
+      <c r="B7">
+        <f>0+5+30+15+5+10+15+5+10+5+20+10+30+10+5+10+15+5+5+5+5+5+10</f>
+        <v/>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>FC Copenhagen</t>
         </is>
       </c>
-      <c r="B7">
-        <f>0</f>
+      <c r="D7">
+        <f>0+5+5+20+5+5+20+5+10+15+10+10+10</f>
+        <v/>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Midtjylland</t>
+        </is>
+      </c>
+      <c r="F7">
+        <f>0+20+30+5+40+20+5+15+10+20+10+10+10</f>
+        <v/>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Brøndby</t>
+        </is>
+      </c>
+      <c r="H7">
+        <f>0+10+5+5+30+10+10+5+10+5+10+20+10+20+10+15+30+10+10+10</f>
         <v/>
       </c>
     </row>
@@ -507,6 +699,33 @@
       </c>
       <c r="B8">
         <f>SUM(B2:B7)</f>
+        <v/>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Total:</t>
+        </is>
+      </c>
+      <c r="D8">
+        <f>SUM(D2:D7)</f>
+        <v/>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Total:</t>
+        </is>
+      </c>
+      <c r="F8">
+        <f>SUM(F2:F7)</f>
+        <v/>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Total:</t>
+        </is>
+      </c>
+      <c r="H8">
+        <f>SUM(H2:H7)</f>
         <v/>
       </c>
     </row>

</xml_diff>